<commit_message>
Update immune receptors distribution
</commit_message>
<xml_diff>
--- a/1_Data Cleaning/gamma-delta (gd) T cell clusters.xlsx
+++ b/1_Data Cleaning/gamma-delta (gd) T cell clusters.xlsx
@@ -1,149 +1,142 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Esmaeil\CeliacProject\CeliacProject\1_Data Cleaning\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3C5F34-7B24-47BD-A6F2-E58111CE8218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
-    <t>cluster</t>
-  </si>
-  <si>
-    <t>total_cells</t>
-  </si>
-  <si>
-    <t>ab</t>
-  </si>
-  <si>
-    <t>Aberrant_ab</t>
-  </si>
-  <si>
-    <t>gd</t>
-  </si>
-  <si>
-    <t>Aberrant_g</t>
-  </si>
-  <si>
-    <t>Act. Tgd</t>
-  </si>
-  <si>
-    <t>Act. plasma IGHA+</t>
-  </si>
-  <si>
-    <t>Act. plasmablast</t>
-  </si>
-  <si>
-    <t>B cells BAFFR+</t>
-  </si>
-  <si>
-    <t>CD4 FTH1+</t>
-  </si>
-  <si>
-    <t>CD4 Trm</t>
-  </si>
-  <si>
-    <t>CD4-CD8-</t>
-  </si>
-  <si>
-    <t>CD4-CD8-IL10+</t>
-  </si>
-  <si>
-    <t>CD8 Mem</t>
-  </si>
-  <si>
-    <t>CD8 Trm</t>
-  </si>
-  <si>
-    <t>Cyt. IEL</t>
-  </si>
-  <si>
-    <t>Homing plasmablast</t>
-  </si>
-  <si>
-    <t>IEL CCL4+</t>
-  </si>
-  <si>
-    <t>IEL GZMK+</t>
-  </si>
-  <si>
-    <t>ILC1/ILC2</t>
-  </si>
-  <si>
-    <t>ILC2/ILTi</t>
-  </si>
-  <si>
-    <t>ILC3</t>
-  </si>
-  <si>
-    <t>Macrophages</t>
-  </si>
-  <si>
-    <t>Mast cells</t>
-  </si>
-  <si>
-    <t>Mature plasma IGHA+</t>
-  </si>
-  <si>
-    <t>Mem B cells</t>
-  </si>
-  <si>
-    <t>NK/Tgd</t>
-  </si>
-  <si>
-    <t>Plasma IGHG+</t>
-  </si>
-  <si>
-    <t>Prolif. IEL</t>
-  </si>
-  <si>
-    <t>T eff. IEL</t>
-  </si>
-  <si>
-    <t>Tfh</t>
-  </si>
-  <si>
-    <t>Tgd CD8+</t>
-  </si>
-  <si>
-    <t>Tgd INSIG1+</t>
-  </si>
-  <si>
-    <t>Th17</t>
-  </si>
-  <si>
-    <t>Tregs</t>
-  </si>
-  <si>
-    <t>Trm IEL</t>
-  </si>
-  <si>
-    <t>nIEL</t>
-  </si>
-  <si>
-    <t>pDC</t>
+    <t xml:space="preserve">cluster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total_cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aberrant_ab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aberrant_g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Act. Tgd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Act. plasma IGHA+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Act. plasmablast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B cells BAFFR+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD4 FTH1+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD4 Trm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD4-CD8-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD4-CD8-IL10+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD8 Mem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD8 Trm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyt. IEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homing plasmablast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IEL CCL4+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IEL GZMK+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILC1/ILC2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILC2/ILTi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILC3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrophages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mast cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mature plasma IGHA+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mem B cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NK/Tgd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plasma IGHG+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prolif. IEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T eff. IEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tfh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tgd CD8+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tgd INSIG1+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Th17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tregs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trm IEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nIEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pDC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -152,18 +145,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -178,23 +165,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -476,16 +453,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD32"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -505,668 +480,668 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" t="n">
         <v>2898</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" t="n">
         <v>182</v>
       </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
         <v>267</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" t="n">
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="n">
         <v>7366</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="n">
         <v>1777</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="n">
         <v>141</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="n">
         <v>5985</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="n">
         <v>1111</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
         <v>17</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="n">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="n">
         <v>17377</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="n">
         <v>6470</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="n">
         <v>19</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="n">
         <v>56</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="n">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="n">
         <v>7318</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="n">
         <v>670</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="n">
         <v>959</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="n">
         <v>29</v>
       </c>
-      <c r="F8">
+      <c r="F8" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="n">
         <v>550</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="n">
         <v>177</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="n">
         <v>2</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="n">
         <v>7635</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="n">
         <v>2021</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="n">
         <v>66</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="n">
         <v>100</v>
       </c>
-      <c r="F10">
+      <c r="F10" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="n">
         <v>6004</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="n">
         <v>3231</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="n">
         <v>46</v>
       </c>
-      <c r="E11">
+      <c r="E11" t="n">
         <v>127</v>
       </c>
-      <c r="F11">
+      <c r="F11" t="n">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="n">
         <v>6923</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="n">
         <v>3669</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
         <v>192</v>
       </c>
-      <c r="F12">
+      <c r="F12" t="n">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="n">
         <v>299</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="n">
         <v>3220</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="n">
         <v>519</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
         <v>45</v>
       </c>
-      <c r="F14">
+      <c r="F14" t="n">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15">
       <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="n">
         <v>11660</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="n">
         <v>3676</v>
       </c>
-      <c r="D15">
+      <c r="D15" t="n">
         <v>152</v>
       </c>
-      <c r="E15">
+      <c r="E15" t="n">
         <v>106</v>
       </c>
-      <c r="F15">
+      <c r="F15" t="n">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="n">
         <v>8242</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="n">
         <v>507</v>
       </c>
-      <c r="D16">
+      <c r="D16" t="n">
         <v>3</v>
       </c>
-      <c r="E16">
+      <c r="E16" t="n">
         <v>54</v>
       </c>
-      <c r="F16">
+      <c r="F16" t="n">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="n">
         <v>128</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="n">
         <v>75</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="n">
         <v>650</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="n">
         <v>36</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
         <v>8</v>
       </c>
-      <c r="F18">
+      <c r="F18" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19">
       <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="n">
         <v>1588</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
       <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="n">
         <v>960</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
       <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="B21">
+      <c r="B21" t="n">
         <v>3615</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
       <c r="A22" t="s">
         <v>26</v>
       </c>
-      <c r="B22">
+      <c r="B22" t="n">
         <v>3084</v>
       </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" t="n">
         <v>3990</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" t="n">
         <v>435</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" t="n">
         <v>5</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" t="n">
         <v>196</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24">
       <c r="A24" t="s">
         <v>28</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="n">
         <v>1506</v>
       </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
-      <c r="B25">
+      <c r="B25" t="n">
         <v>2010</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="n">
         <v>979</v>
       </c>
-      <c r="D25">
+      <c r="D25" t="n">
         <v>5</v>
       </c>
-      <c r="E25">
+      <c r="E25" t="n">
         <v>88</v>
       </c>
-      <c r="F25">
+      <c r="F25" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26">
       <c r="A26" t="s">
         <v>30</v>
       </c>
-      <c r="B26">
+      <c r="B26" t="n">
         <v>3021</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="n">
         <v>702</v>
       </c>
-      <c r="D26">
+      <c r="D26" t="n">
         <v>576</v>
       </c>
-      <c r="E26">
+      <c r="E26" t="n">
         <v>10</v>
       </c>
-      <c r="F26">
+      <c r="F26" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27">
       <c r="A27" t="s">
         <v>31</v>
       </c>
-      <c r="B27">
+      <c r="B27" t="n">
         <v>6537</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="n">
         <v>2938</v>
       </c>
-      <c r="D27">
+      <c r="D27" t="n">
         <v>4</v>
       </c>
-      <c r="E27">
+      <c r="E27" t="n">
         <v>15</v>
       </c>
-      <c r="F27">
+      <c r="F27" t="n">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="28">
+      <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" t="n">
         <v>12265</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" t="n">
         <v>2843</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" t="n">
         <v>3</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" t="n">
         <v>647</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28" t="n">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="29">
+      <c r="A29" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" t="n">
         <v>1804</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" t="n">
         <v>348</v>
       </c>
-      <c r="D29" s="1">
-        <v>0</v>
-      </c>
-      <c r="E29" s="1">
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
         <v>627</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" t="n">
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30">
       <c r="A30" t="s">
         <v>34</v>
       </c>
-      <c r="B30">
+      <c r="B30" t="n">
         <v>15640</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="n">
         <v>5127</v>
       </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
         <v>36</v>
       </c>
-      <c r="F30">
+      <c r="F30" t="n">
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31">
       <c r="A31" t="s">
         <v>35</v>
       </c>
-      <c r="B31">
+      <c r="B31" t="n">
         <v>4891</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="n">
         <v>2196</v>
       </c>
-      <c r="D31">
+      <c r="D31" t="n">
         <v>1</v>
       </c>
-      <c r="E31">
+      <c r="E31" t="n">
         <v>5</v>
       </c>
-      <c r="F31">
+      <c r="F31" t="n">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="32">
+      <c r="A32" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" t="n">
         <v>10961</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" t="n">
         <v>2723</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" t="n">
         <v>3</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32" t="n">
         <v>1259</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32" t="n">
         <v>834</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33">
       <c r="A33" t="s">
         <v>37</v>
       </c>
-      <c r="B33">
+      <c r="B33" t="n">
         <v>1320</v>
       </c>
-      <c r="C33">
+      <c r="C33" t="n">
         <v>420</v>
       </c>
-      <c r="D33">
+      <c r="D33" t="n">
         <v>1</v>
       </c>
-      <c r="E33">
+      <c r="E33" t="n">
         <v>72</v>
       </c>
-      <c r="F33">
+      <c r="F33" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34">
       <c r="A34" t="s">
         <v>38</v>
       </c>
-      <c r="B34">
+      <c r="B34" t="n">
         <v>145</v>
       </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34">
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>